<commit_message>
Dramatically removed hard-coding and classes coupling
Version 0.2, still not playable.
Fixed several fatal bugs
Removed many hard-codings, thanks to Shenbo's pointing out.
Improved design, deduced coupling.
Better output.
</commit_message>
<xml_diff>
--- a/helperResource/Cluedo.xlsx
+++ b/helperResource/Cluedo.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="91">
   <si>
     <t>┌</t>
   </si>
@@ -226,6 +226,154 @@
   </si>
   <si>
     <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kitchen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ballroom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>csty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>billard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>library</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lounge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dining room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23,19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23,21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20,11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20,12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displaying tiles:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -279,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +437,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -465,7 +619,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -853,7 +1016,7 @@
   <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A3" sqref="A3:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -864,38 +1027,39 @@
     <col min="27" max="27" width="3.25" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="34" width="2.75" style="1"/>
     <col min="35" max="35" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="41" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="5.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="16384" width="2.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="C1" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
+      <c r="C1" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
     </row>
     <row r="2" spans="1:41" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C2" s="2">
@@ -996,8 +1160,8 @@
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>52</v>
+      <c r="A3" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -1094,7 +1258,7 @@
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1181,7 +1345,7 @@
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1268,7 +1432,7 @@
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -1326,10 +1490,10 @@
       <c r="U6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
       <c r="Z6" s="16" t="s">
         <v>3</v>
       </c>
@@ -1359,23 +1523,23 @@
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="D7" s="28">
+        <v>1</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -1420,8 +1584,8 @@
       <c r="V7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W7" s="3"/>
-      <c r="X7" s="4"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="28"/>
       <c r="Y7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1433,7 +1597,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -1443,10 +1607,10 @@
       <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1467,13 +1631,13 @@
       <c r="L8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="4" t="s">
+      <c r="M8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="28" t="s">
         <v>29</v>
       </c>
       <c r="P8" s="4" t="s">
@@ -1512,9 +1676,12 @@
       <c r="AA8" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI8" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -1551,13 +1718,13 @@
       <c r="M9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="4" t="s">
+      <c r="N9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Q9" s="4" t="s">
@@ -1593,9 +1760,21 @@
       <c r="AA9" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -1608,7 +1787,7 @@
       <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="27" t="s">
         <v>29</v>
       </c>
       <c r="G10" s="26" t="s">
@@ -1674,9 +1853,21 @@
       <c r="AA10" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2">
         <v>8</v>
       </c>
@@ -1755,9 +1946,21 @@
       <c r="AA11" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2">
         <v>9</v>
       </c>
@@ -1822,13 +2025,13 @@
         <v>37</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="Z12" s="16" t="s">
         <v>3</v>
@@ -1836,9 +2039,21 @@
       <c r="AA12" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="2">
         <v>10</v>
       </c>
@@ -1899,15 +2114,9 @@
       <c r="U13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X13" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="16" t="s">
         <v>3</v>
@@ -1918,9 +2127,21 @@
       <c r="AE13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="AI13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2">
         <v>11</v>
       </c>
@@ -1981,9 +2202,9 @@
       <c r="U14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4" t="s">
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Y14" s="4" t="s">
@@ -1995,9 +2216,21 @@
       <c r="AA14" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2">
         <v>12</v>
       </c>
@@ -2074,22 +2307,34 @@
       <c r="AA15" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL15" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2">
         <v>13</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -2145,9 +2390,21 @@
       <c r="AA16" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
       <c r="B17" s="2">
         <v>14</v>
       </c>
@@ -2157,13 +2414,13 @@
       <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -2226,9 +2483,21 @@
       <c r="AA17" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AI17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
       <c r="B18" s="2">
         <v>15</v>
       </c>
@@ -2308,8 +2577,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A19" s="29"/>
       <c r="B19" s="2">
         <v>16</v>
       </c>
@@ -2368,18 +2637,10 @@
         <v>18</v>
       </c>
       <c r="U19" s="4"/>
-      <c r="V19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="W19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y19" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="V19" s="4"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
       <c r="Z19" s="16" t="s">
         <v>3</v>
       </c>
@@ -2387,8 +2648,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A20" s="29"/>
       <c r="B20" s="2">
         <v>17</v>
       </c>
@@ -2439,13 +2700,13 @@
       <c r="U20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="V20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="W20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="X20" s="4" t="s">
+      <c r="V20" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="W20" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X20" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Y20" s="3" t="s">
@@ -2458,8 +2719,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A21" s="29"/>
       <c r="B21" s="2">
         <v>18</v>
       </c>
@@ -2539,8 +2800,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
       <c r="B22" s="2">
         <v>19</v>
       </c>
@@ -2610,8 +2871,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
       <c r="B23" s="2">
         <v>20</v>
       </c>
@@ -2645,13 +2906,13 @@
       <c r="L23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O23" s="4" t="s">
+      <c r="M23" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="27" t="s">
         <v>29</v>
       </c>
       <c r="P23" s="4" t="s">
@@ -2681,8 +2942,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
       <c r="B24" s="2">
         <v>21</v>
       </c>
@@ -2716,13 +2977,13 @@
       <c r="L24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="4" t="s">
+      <c r="M24" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="28" t="s">
         <v>29</v>
       </c>
       <c r="P24" s="4" t="s">
@@ -2762,21 +3023,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A25" s="29"/>
       <c r="B25" s="2">
         <v>22</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="4" t="s">
+      <c r="D25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="28" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -2800,13 +3061,13 @@
       <c r="M25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="4" t="s">
+      <c r="N25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="O25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="P25" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Q25" s="3" t="s">
@@ -2843,8 +3104,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A26" s="29"/>
       <c r="B26" s="2">
         <v>23</v>
       </c>
@@ -2854,13 +3115,13 @@
       <c r="D26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="E26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -2905,16 +3166,16 @@
       <c r="U26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="V26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="W26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="X26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y26" s="4" t="s">
+      <c r="V26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="W26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y26" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Z26" s="16" t="s">
@@ -2924,8 +3185,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A27" s="29"/>
       <c r="B27" s="2">
         <v>24</v>
       </c>

</xml_diff>